<commit_message>
Survey Analysis script and exports/plots
</commit_message>
<xml_diff>
--- a/survey_results.xlsx
+++ b/survey_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/badd34f802a75890/Dokumente/Office/Master/4. Semester/AS IS^0DT/Paper/ASISaDT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D2C1C58-3A61-4761-A442-11BB8AAEA0B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{0D2C1C58-3A61-4761-A442-11BB8AAEA0B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3E2456B4-D0BE-47B0-A3F2-F4048D343D17}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96472D23-079C-4042-AF09-E9D5A93651C9}"/>
   </bookViews>
@@ -826,7 +826,7 @@
   <dimension ref="A1:W55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
latest changes and added survey as html documenty:
</commit_message>
<xml_diff>
--- a/survey_results.xlsx
+++ b/survey_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/badd34f802a75890/Dokumente/Office/Master/4. Semester/AS IS^0DT/Paper/ASISaDT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{0D2C1C58-3A61-4761-A442-11BB8AAEA0B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3E2456B4-D0BE-47B0-A3F2-F4048D343D17}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{0D2C1C58-3A61-4761-A442-11BB8AAEA0B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{82C49EA3-9707-428E-8FA3-66DD3C2330A6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96472D23-079C-4042-AF09-E9D5A93651C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{96472D23-079C-4042-AF09-E9D5A93651C9}"/>
   </bookViews>
   <sheets>
     <sheet name="survey_results" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="97">
   <si>
     <t>id</t>
   </si>
@@ -337,10 +337,6 @@
     <t>wird die Akzeptanz bei Nutzern erhöhen</t>
   </si>
   <si>
-    <t>Effizienz
-Benutzerfreundlicher</t>
-  </si>
-  <si>
     <t>Effizienz Steuerung</t>
   </si>
   <si>
@@ -348,6 +344,9 @@
   </si>
   <si>
     <t>Effinzienz, Fahrgasströme, Steuerung</t>
+  </si>
+  <si>
+    <t>Effizienz Benutzerfreundlicher</t>
   </si>
 </sst>
 </file>
@@ -825,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D34EDD6-A39C-4342-9A5B-84C53C1C02E5}">
   <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="W49" sqref="W49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3498,7 +3497,7 @@
         <v>24</v>
       </c>
       <c r="W38" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
@@ -4066,7 +4065,7 @@
         <v>30</v>
       </c>
       <c r="W46" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
@@ -4137,7 +4136,7 @@
         <v>24</v>
       </c>
       <c r="W47" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
@@ -4279,7 +4278,7 @@
         <v>24</v>
       </c>
       <c r="W49" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.25">
@@ -4659,8 +4658,9 @@
       <c r="M55" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="N55" s="2" t="s">
-        <v>38</v>
+      <c r="N55" s="2">
+        <f>53 - COUNTIF(N2:N54,N54)</f>
+        <v>17</v>
       </c>
       <c r="O55" s="2" t="s">
         <v>38</v>
@@ -4674,8 +4674,9 @@
       <c r="R55" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S55" s="2" t="s">
-        <v>38</v>
+      <c r="S55" s="2">
+        <f>53 - COUNTIF(S2:S54,S54)</f>
+        <v>17</v>
       </c>
       <c r="T55" s="2" t="s">
         <v>38</v>
@@ -4686,8 +4687,9 @@
       <c r="V55" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="W55" s="2" t="s">
-        <v>38</v>
+      <c r="W55" s="2">
+        <f>53-COUNTIF(W2:W54,W54)</f>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>